<commit_message>
Giving the multiprocessing.Process object as a argument
</commit_message>
<xml_diff>
--- a/DailyWorks.xlsx
+++ b/DailyWorks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Time</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Test 0</t>
+  </si>
+  <si>
+    <t>Test 1 Bro</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +478,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>0.58333333333333337</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
@@ -527,6 +530,14 @@
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>0.59236111111111112</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made the video for this
</commit_message>
<xml_diff>
--- a/DailyWorks.xlsx
+++ b/DailyWorks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Time</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Test 1 Bro</t>
+  </si>
+  <si>
+    <t>Go for the dinner by shutting down pc</t>
   </si>
 </sst>
 </file>
@@ -71,14 +74,14 @@
       <b/>
       <i/>
       <u/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +91,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -104,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -112,20 +121,23 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,63 +452,63 @@
     <col min="2" max="2" width="46.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>0.5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>0.52083333333333337</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>0.59027777777777779</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>0.61805555555555558</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>0.64583333333333337</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -509,15 +521,15 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>0.72916666666666663</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>0.67291666666666661</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -525,7 +537,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>0.67361111111111116</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -538,6 +550,14 @@
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>0.8125</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put all my daily task regularly
</commit_message>
<xml_diff>
--- a/DailyWorks.xlsx
+++ b/DailyWorks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Time</t>
   </si>
@@ -25,15 +25,6 @@
     <t>Chek Emails, Discord, and all social Media accounts</t>
   </si>
   <si>
-    <t>Fix some Bugs of Alice</t>
-  </si>
-  <si>
-    <t>Have a ATL Session to attent</t>
-  </si>
-  <si>
-    <t>Work on Alice</t>
-  </si>
-  <si>
     <t>Wanna solve 2 to 3 questions of codeforces</t>
   </si>
   <si>
@@ -49,22 +40,37 @@
     <t>Alice Testing and bug fixing</t>
   </si>
   <si>
-    <t>Test 0</t>
-  </si>
-  <si>
-    <t>Test 1 Bro</t>
-  </si>
-  <si>
     <t>Go for the dinner by shutting down pc</t>
   </si>
   <si>
-    <t xml:space="preserve">Test 2 </t>
-  </si>
-  <si>
-    <t>Test 5</t>
-  </si>
-  <si>
-    <t>Test 4</t>
+    <t>Start to work on Alice</t>
+  </si>
+  <si>
+    <t>Have a break, Go for lunch</t>
+  </si>
+  <si>
+    <t>Contribution in Python-Discord</t>
+  </si>
+  <si>
+    <t>Time pass on python discord by helping others</t>
+  </si>
+  <si>
+    <t>ATL Session</t>
+  </si>
+  <si>
+    <t>Playing Krunker online Game</t>
+  </si>
+  <si>
+    <t>Start Solving the Practise sets of python</t>
+  </si>
+  <si>
+    <t>Read Books</t>
+  </si>
+  <si>
+    <t>Read core python book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scroll Instagram and post 1 python trick </t>
   </si>
 </sst>
 </file>
@@ -452,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +495,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -497,7 +503,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -505,7 +511,7 @@
         <v>0.59722222222222221</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -513,7 +519,7 @@
         <v>0.61805555555555558</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,7 +527,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -529,7 +535,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -537,7 +543,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -545,28 +551,28 @@
         <v>0.67291666666666661</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>0.67361111111111116</v>
+        <v>0.8125</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>0.59236111111111112</v>
+      <c r="A13" s="9">
+        <v>0.71875</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>0.8125</v>
+      <c r="A14" s="9">
+        <v>0.79166666666666663</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -574,26 +580,42 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
-        <v>0.1076388888888889</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>0.10416666666666667</v>
+      <c r="A16" s="6">
+        <v>0.90625</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>9.7916666666666666E-2</v>
+      <c r="A17" s="6">
+        <v>0.95833333333333337</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a bug found while using muliprocessing
</commit_message>
<xml_diff>
--- a/DailyWorks.xlsx
+++ b/DailyWorks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Time</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">Scroll Instagram and post 1 python trick </t>
+  </si>
+  <si>
+    <t>Test 0</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,6 +621,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>0.63750000000000007</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>